<commit_message>
Updated: PokeMoves spreadsheet, PokeMoves data table, references to PokeMoves data table, moveStruct variables, & battle widget for changes to MoveStruct. Added stat stage adjustments to battle widget.
</commit_message>
<xml_diff>
--- a/PokeMoves.xlsx
+++ b/PokeMoves.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beerb\My Games\Get-Dem-Pokes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CFA4FD-9995-464E-96D8-7BCEF3DD7365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E88DF5-CD8D-40AA-910D-3350A3A1A591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68355" yWindow="18570" windowWidth="18045" windowHeight="8160" tabRatio="133" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Poke_Moves_-_Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PokeMoves" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -901,9 +901,6 @@
     <t>Recharge</t>
   </si>
   <si>
-    <t>Descrption</t>
-  </si>
-  <si>
     <t xml:space="preserve"> is storing energy</t>
   </si>
   <si>
@@ -919,9 +916,6 @@
     <t>Typeless</t>
   </si>
   <si>
-    <t>1,3</t>
-  </si>
-  <si>
     <t>SleepChance</t>
   </si>
   <si>
@@ -947,12 +941,21 @@
   </si>
   <si>
     <t>CriticalStage</t>
+  </si>
+  <si>
+    <t>(1,3)</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\(0\)"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1499,7 +1502,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1511,6 +1514,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1869,8 +1881,8 @@
   <dimension ref="A1:AH166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AL1048576"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F167" sqref="F167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1884,9 +1896,9 @@
     <col min="8" max="8" width="9.08984375" customWidth="1"/>
     <col min="9" max="9" width="10.81640625" customWidth="1"/>
     <col min="10" max="10" width="6.36328125" customWidth="1"/>
-    <col min="11" max="11" width="7.36328125" customWidth="1"/>
+    <col min="11" max="11" width="7.08984375" customWidth="1"/>
     <col min="12" max="12" width="18.81640625" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="12" customWidth="1"/>
     <col min="14" max="14" width="6.90625" customWidth="1"/>
     <col min="15" max="15" width="4.08984375" customWidth="1"/>
     <col min="16" max="17" width="9.6328125" customWidth="1"/>
@@ -1935,7 +1947,7 @@
         <v>275</v>
       </c>
       <c r="I1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J1" t="s">
         <v>277</v>
@@ -1944,22 +1956,22 @@
         <v>287</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="M1" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="N1" t="s">
         <v>278</v>
       </c>
       <c r="O1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P1" t="s">
         <v>281</v>
       </c>
       <c r="Q1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="R1" t="s">
         <v>282</v>
@@ -1983,7 +1995,7 @@
         <v>280</v>
       </c>
       <c r="Y1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="Z1" t="s">
         <v>279</v>
@@ -2001,13 +2013,13 @@
         <v>288</v>
       </c>
       <c r="AE1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AF1" t="s">
         <v>276</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>289</v>
@@ -2030,7 +2042,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G2">
         <v>25</v>
@@ -2050,7 +2062,7 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="12">
         <v>0</v>
       </c>
       <c r="N2">
@@ -2131,7 +2143,7 @@
         <v>40</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <v>30</v>
@@ -2151,7 +2163,7 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="13">
         <v>4</v>
       </c>
       <c r="N3">
@@ -2252,7 +2264,7 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="12">
         <v>2</v>
       </c>
       <c r="N4">
@@ -2353,7 +2365,7 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="12">
         <v>5</v>
       </c>
       <c r="N5">
@@ -2454,7 +2466,7 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="12">
         <v>4</v>
       </c>
       <c r="N6">
@@ -2535,7 +2547,7 @@
         <v>65</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G7">
         <v>20</v>
@@ -2555,7 +2567,7 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="12">
         <v>1</v>
       </c>
       <c r="N7">
@@ -2636,7 +2648,7 @@
         <v>15</v>
       </c>
       <c r="F8">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -2656,7 +2668,7 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="12">
         <v>0</v>
       </c>
       <c r="N8">
@@ -2757,7 +2769,7 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="12">
         <v>2</v>
       </c>
       <c r="N9">
@@ -2838,7 +2850,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3">
         <v>10</v>
@@ -2858,7 +2870,7 @@
       <c r="L10" s="3">
         <v>0</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="14">
         <v>0</v>
       </c>
       <c r="N10" s="3">
@@ -2916,7 +2928,7 @@
         <v>3</v>
       </c>
       <c r="AF10" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AG10" s="3" t="s">
         <v>29</v>
@@ -2942,7 +2954,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="2">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G11" s="2">
         <v>20</v>
@@ -2962,7 +2974,7 @@
       <c r="L11" s="2">
         <v>0</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="15">
         <v>0</v>
       </c>
       <c r="N11" s="2">
@@ -3020,7 +3032,7 @@
         <v>5</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AG11" s="2" t="s">
         <v>31</v>
@@ -3046,7 +3058,7 @@
         <v>60</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G12">
         <v>25</v>
@@ -3066,7 +3078,7 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="12">
         <v>0</v>
       </c>
       <c r="N12">
@@ -3147,7 +3159,7 @@
         <v>110</v>
       </c>
       <c r="F13">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="G13">
         <v>5</v>
@@ -3167,7 +3179,7 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="12">
         <v>0</v>
       </c>
       <c r="N13">
@@ -3248,7 +3260,7 @@
         <v>85</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G14">
         <v>15</v>
@@ -3268,7 +3280,7 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="12">
         <v>0</v>
       </c>
       <c r="N14">
@@ -3349,7 +3361,7 @@
         <v>65</v>
       </c>
       <c r="F15">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G15">
         <v>20</v>
@@ -3369,7 +3381,7 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="12">
         <v>0</v>
       </c>
       <c r="N15">
@@ -3450,7 +3462,7 @@
         <v>50</v>
       </c>
       <c r="F16">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G16">
         <v>10</v>
@@ -3470,7 +3482,7 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="12">
         <v>0</v>
       </c>
       <c r="N16">
@@ -3551,7 +3563,7 @@
         <v>40</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G17">
         <v>30</v>
@@ -3571,7 +3583,7 @@
       <c r="L17">
         <v>1</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="12">
         <v>5</v>
       </c>
       <c r="N17">
@@ -3652,7 +3664,7 @@
         <v>65</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G18">
         <v>20</v>
@@ -3672,7 +3684,7 @@
       <c r="L18">
         <v>1</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="12">
         <v>5</v>
       </c>
       <c r="N18">
@@ -3753,7 +3765,7 @@
         <v>35</v>
       </c>
       <c r="F19" s="5">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G19" s="5">
         <v>15</v>
@@ -3771,9 +3783,9 @@
         <v>0</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="M19" s="5">
+        <v>299</v>
+      </c>
+      <c r="M19" s="16">
         <v>0</v>
       </c>
       <c r="N19" s="5">
@@ -3831,7 +3843,7 @@
         <v>5</v>
       </c>
       <c r="AF19" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AG19" s="5" t="s">
         <v>48</v>
@@ -3857,7 +3869,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="6">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G20" s="6">
         <v>15</v>
@@ -3877,7 +3889,7 @@
       <c r="L20" s="6">
         <v>0</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="17">
         <v>0</v>
       </c>
       <c r="N20" s="6">
@@ -3958,7 +3970,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G21">
         <v>10</v>
@@ -3978,7 +3990,7 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="12">
         <v>0</v>
       </c>
       <c r="N21">
@@ -4059,7 +4071,7 @@
         <v>50</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G22">
         <v>25</v>
@@ -4079,7 +4091,7 @@
       <c r="L22">
         <v>0</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="12">
         <v>0</v>
       </c>
       <c r="N22">
@@ -4160,7 +4172,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G23" s="6">
         <v>35</v>
@@ -4180,7 +4192,7 @@
       <c r="L23" s="6">
         <v>1</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="17">
         <v>5</v>
       </c>
       <c r="N23" s="6">
@@ -4281,7 +4293,7 @@
       <c r="L24" s="2">
         <v>0</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="15">
         <v>0</v>
       </c>
       <c r="N24" s="2">
@@ -4353,7 +4365,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>25</v>
@@ -4362,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G25" s="2">
         <v>20</v>
@@ -4382,7 +4394,7 @@
       <c r="L25" s="2">
         <v>0</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="15">
         <v>0</v>
       </c>
       <c r="N25" s="2">
@@ -4463,7 +4475,7 @@
         <v>100</v>
       </c>
       <c r="F26">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G26">
         <v>10</v>
@@ -4483,7 +4495,7 @@
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="12">
         <v>0</v>
       </c>
       <c r="N26">
@@ -4564,7 +4576,7 @@
         <v>50</v>
       </c>
       <c r="F27">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="G27">
         <v>30</v>
@@ -4584,7 +4596,7 @@
       <c r="L27">
         <v>0</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="12">
         <v>0</v>
       </c>
       <c r="N27">
@@ -4685,7 +4697,7 @@
       <c r="L28">
         <v>0</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="12">
         <v>2</v>
       </c>
       <c r="N28">
@@ -4766,7 +4778,7 @@
         <v>80</v>
       </c>
       <c r="F29" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G29" s="2">
         <v>10</v>
@@ -4786,7 +4798,7 @@
       <c r="L29" s="2">
         <v>0</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="15">
         <v>0</v>
       </c>
       <c r="N29" s="2">
@@ -4867,7 +4879,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G30" s="2">
         <v>20</v>
@@ -4887,7 +4899,7 @@
       <c r="L30" s="2">
         <v>0</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="15">
         <v>0</v>
       </c>
       <c r="N30" s="2">
@@ -4968,7 +4980,7 @@
         <v>70</v>
       </c>
       <c r="F31" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G31" s="6">
         <v>10</v>
@@ -4988,7 +5000,7 @@
       <c r="L31" s="6">
         <v>0</v>
       </c>
-      <c r="M31" s="6">
+      <c r="M31" s="17">
         <v>0</v>
       </c>
       <c r="N31" s="6">
@@ -5069,7 +5081,7 @@
         <v>30</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G32">
         <v>30</v>
@@ -5089,7 +5101,7 @@
       <c r="L32">
         <v>0</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="12">
         <v>0</v>
       </c>
       <c r="N32">
@@ -5170,7 +5182,7 @@
         <v>15</v>
       </c>
       <c r="F33" s="6">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G33" s="6">
         <v>10</v>
@@ -5190,7 +5202,7 @@
       <c r="L33" s="6">
         <v>0</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M33" s="17">
         <v>0</v>
       </c>
       <c r="N33" s="6">
@@ -5291,7 +5303,7 @@
       <c r="L34">
         <v>0</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="12">
         <v>7</v>
       </c>
       <c r="N34">
@@ -5372,7 +5384,7 @@
         <v>120</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G35">
         <v>15</v>
@@ -5392,7 +5404,7 @@
       <c r="L35">
         <v>0</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="12">
         <v>0</v>
       </c>
       <c r="N35">
@@ -5473,7 +5485,7 @@
         <v>40</v>
       </c>
       <c r="F36" s="5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G36" s="5">
         <v>10</v>
@@ -5493,7 +5505,7 @@
       <c r="L36" s="5">
         <v>0</v>
       </c>
-      <c r="M36" s="5">
+      <c r="M36" s="16">
         <v>0</v>
       </c>
       <c r="N36" s="5">
@@ -5574,7 +5586,7 @@
         <v>100</v>
       </c>
       <c r="F37" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G37" s="2">
         <v>15</v>
@@ -5594,7 +5606,7 @@
       <c r="L37" s="2">
         <v>0</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37" s="15">
         <v>0</v>
       </c>
       <c r="N37" s="2">
@@ -5675,7 +5687,7 @@
         <v>80</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G38">
         <v>20</v>
@@ -5695,7 +5707,7 @@
       <c r="L38">
         <v>0</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="12">
         <v>0</v>
       </c>
       <c r="N38">
@@ -5773,7 +5785,7 @@
         <v>100</v>
       </c>
       <c r="F39" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G39" s="2">
         <v>10</v>
@@ -5793,7 +5805,7 @@
       <c r="L39" s="2">
         <v>0</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39" s="15">
         <v>0</v>
       </c>
       <c r="N39" s="2">
@@ -5874,7 +5886,7 @@
         <v>100</v>
       </c>
       <c r="F40" s="6">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="G40" s="6">
         <v>10</v>
@@ -5894,7 +5906,7 @@
       <c r="L40" s="6">
         <v>0</v>
       </c>
-      <c r="M40" s="6">
+      <c r="M40" s="17">
         <v>0</v>
       </c>
       <c r="N40" s="6">
@@ -5972,7 +5984,7 @@
         <v>40</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G41">
         <v>25</v>
@@ -5992,7 +6004,7 @@
       <c r="L41">
         <v>0</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="12">
         <v>0</v>
       </c>
       <c r="N41">
@@ -6073,7 +6085,7 @@
         <v>250</v>
       </c>
       <c r="F42" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G42" s="2">
         <v>5</v>
@@ -6093,7 +6105,7 @@
       <c r="L42" s="2">
         <v>0</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42" s="15">
         <v>0</v>
       </c>
       <c r="N42" s="2">
@@ -6174,7 +6186,7 @@
         <v>110</v>
       </c>
       <c r="F43">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -6194,7 +6206,7 @@
       <c r="L43">
         <v>0</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="12">
         <v>0</v>
       </c>
       <c r="N43">
@@ -6275,7 +6287,7 @@
         <v>75</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G44">
         <v>15</v>
@@ -6295,7 +6307,7 @@
       <c r="L44">
         <v>0</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="12">
         <v>0</v>
       </c>
       <c r="N44">
@@ -6376,7 +6388,7 @@
         <v>35</v>
       </c>
       <c r="F45" s="2">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G45" s="2">
         <v>15</v>
@@ -6396,7 +6408,7 @@
       <c r="L45" s="2">
         <v>0</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="15">
         <v>0</v>
       </c>
       <c r="N45" s="2">
@@ -6477,7 +6489,7 @@
         <v>-1</v>
       </c>
       <c r="F46" s="2">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="G46" s="2">
         <v>5</v>
@@ -6497,7 +6509,7 @@
       <c r="L46" s="2">
         <v>0</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="15">
         <v>0</v>
       </c>
       <c r="N46" s="2">
@@ -6578,7 +6590,7 @@
         <v>90</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G47">
         <v>15</v>
@@ -6598,7 +6610,7 @@
       <c r="L47">
         <v>0</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="12">
         <v>0</v>
       </c>
       <c r="N47">
@@ -6679,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G48">
         <v>20</v>
@@ -6699,7 +6711,7 @@
       <c r="L48">
         <v>1</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="12">
         <v>6</v>
       </c>
       <c r="N48">
@@ -6780,7 +6792,7 @@
         <v>90</v>
       </c>
       <c r="F49" s="4">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="G49" s="4">
         <v>15</v>
@@ -6800,7 +6812,7 @@
       <c r="L49" s="4">
         <v>0</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M49" s="18">
         <v>0</v>
       </c>
       <c r="N49" s="4">
@@ -6901,7 +6913,7 @@
       <c r="L50">
         <v>0</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="12">
         <v>8</v>
       </c>
       <c r="N50">
@@ -6982,7 +6994,7 @@
         <v>15</v>
       </c>
       <c r="F51">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G51">
         <v>20</v>
@@ -7002,7 +7014,7 @@
       <c r="L51">
         <v>0</v>
       </c>
-      <c r="M51">
+      <c r="M51" s="12">
         <v>0</v>
       </c>
       <c r="N51">
@@ -7083,7 +7095,7 @@
         <v>18</v>
       </c>
       <c r="F52">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="G52">
         <v>15</v>
@@ -7103,7 +7115,7 @@
       <c r="L52">
         <v>0</v>
       </c>
-      <c r="M52">
+      <c r="M52" s="12">
         <v>0</v>
       </c>
       <c r="N52">
@@ -7184,7 +7196,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G53">
         <v>30</v>
@@ -7204,7 +7216,7 @@
       <c r="L53">
         <v>0</v>
       </c>
-      <c r="M53">
+      <c r="M53" s="12">
         <v>0</v>
       </c>
       <c r="N53">
@@ -7285,7 +7297,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G54">
         <v>40</v>
@@ -7305,7 +7317,7 @@
       <c r="L54">
         <v>1</v>
       </c>
-      <c r="M54">
+      <c r="M54" s="12">
         <v>1</v>
       </c>
       <c r="N54">
@@ -7406,8 +7418,8 @@
       <c r="L55">
         <v>0</v>
       </c>
-      <c r="M55" t="s">
-        <v>299</v>
+      <c r="M55" s="12" t="s">
+        <v>307</v>
       </c>
       <c r="N55">
         <v>0</v>
@@ -7487,7 +7499,7 @@
         <v>-1</v>
       </c>
       <c r="F56" s="2">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="G56" s="2">
         <v>5</v>
@@ -7507,7 +7519,7 @@
       <c r="L56" s="2">
         <v>0</v>
       </c>
-      <c r="M56" s="2">
+      <c r="M56" s="15">
         <v>0</v>
       </c>
       <c r="N56" s="2">
@@ -7588,7 +7600,7 @@
         <v>40</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G57">
         <v>35</v>
@@ -7608,7 +7620,7 @@
       <c r="L57">
         <v>0</v>
       </c>
-      <c r="M57">
+      <c r="M57" s="12">
         <v>0</v>
       </c>
       <c r="N57">
@@ -7709,7 +7721,7 @@
       <c r="L58">
         <v>0</v>
       </c>
-      <c r="M58">
+      <c r="M58" s="12">
         <v>2</v>
       </c>
       <c r="N58">
@@ -7810,7 +7822,7 @@
       <c r="L59" s="2">
         <v>0</v>
       </c>
-      <c r="M59" s="2">
+      <c r="M59" s="15">
         <v>0</v>
       </c>
       <c r="N59" s="2">
@@ -7891,7 +7903,7 @@
         <v>70</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G60">
         <v>15</v>
@@ -7911,7 +7923,7 @@
       <c r="L60">
         <v>0</v>
       </c>
-      <c r="M60">
+      <c r="M60" s="12">
         <v>0</v>
       </c>
       <c r="N60">
@@ -7992,7 +8004,7 @@
         <v>130</v>
       </c>
       <c r="F61" s="2">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G61" s="2">
         <v>10</v>
@@ -8012,7 +8024,7 @@
       <c r="L61" s="2">
         <v>0</v>
       </c>
-      <c r="M61" s="2">
+      <c r="M61" s="15">
         <v>0</v>
       </c>
       <c r="N61" s="2">
@@ -8093,7 +8105,7 @@
         <v>65</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G62">
         <v>25</v>
@@ -8113,7 +8125,7 @@
       <c r="L62">
         <v>0</v>
       </c>
-      <c r="M62">
+      <c r="M62" s="12">
         <v>0</v>
       </c>
       <c r="N62">
@@ -8191,7 +8203,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="G63" s="2">
         <v>5</v>
@@ -8211,7 +8223,7 @@
       <c r="L63" s="2">
         <v>0</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="15">
         <v>0</v>
       </c>
       <c r="N63" s="2">
@@ -8292,7 +8304,7 @@
         <v>110</v>
       </c>
       <c r="F64">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="G64">
         <v>5</v>
@@ -8312,7 +8324,7 @@
       <c r="L64">
         <v>0</v>
       </c>
-      <c r="M64">
+      <c r="M64" s="12">
         <v>0</v>
       </c>
       <c r="N64">
@@ -8390,7 +8402,7 @@
         <v>150</v>
       </c>
       <c r="F65">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G65">
         <v>5</v>
@@ -8410,7 +8422,7 @@
       <c r="L65">
         <v>0</v>
       </c>
-      <c r="M65">
+      <c r="M65" s="12">
         <v>0</v>
       </c>
       <c r="N65">
@@ -8491,7 +8503,7 @@
         <v>80</v>
       </c>
       <c r="F66">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G66">
         <v>15</v>
@@ -8511,7 +8523,7 @@
       <c r="L66">
         <v>0</v>
       </c>
-      <c r="M66">
+      <c r="M66" s="12">
         <v>0</v>
       </c>
       <c r="N66">
@@ -8592,7 +8604,7 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="G67">
         <v>20</v>
@@ -8612,7 +8624,7 @@
       <c r="L67">
         <v>0</v>
       </c>
-      <c r="M67">
+      <c r="M67" s="12">
         <v>0</v>
       </c>
       <c r="N67">
@@ -8693,7 +8705,7 @@
         <v>90</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G68">
         <v>10</v>
@@ -8713,7 +8725,7 @@
       <c r="L68">
         <v>0</v>
       </c>
-      <c r="M68">
+      <c r="M68" s="12">
         <v>0</v>
       </c>
       <c r="N68">
@@ -8794,7 +8806,7 @@
         <v>75</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G69">
         <v>15</v>
@@ -8814,7 +8826,7 @@
       <c r="L69">
         <v>0</v>
       </c>
-      <c r="M69">
+      <c r="M69" s="12">
         <v>0</v>
       </c>
       <c r="N69">
@@ -8895,7 +8907,7 @@
         <v>100</v>
       </c>
       <c r="F70" s="6">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="G70" s="6">
         <v>10</v>
@@ -8915,7 +8927,7 @@
       <c r="L70" s="6">
         <v>0</v>
       </c>
-      <c r="M70" s="6">
+      <c r="M70" s="17">
         <v>0</v>
       </c>
       <c r="N70" s="6">
@@ -8996,7 +9008,7 @@
         <v>50</v>
       </c>
       <c r="F71" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G71" s="6">
         <v>25</v>
@@ -9016,7 +9028,7 @@
       <c r="L71" s="6">
         <v>0</v>
       </c>
-      <c r="M71" s="6">
+      <c r="M71" s="17">
         <v>0</v>
       </c>
       <c r="N71" s="6">
@@ -9097,7 +9109,7 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="G72">
         <v>15</v>
@@ -9117,7 +9129,7 @@
       <c r="L72">
         <v>1</v>
       </c>
-      <c r="M72">
+      <c r="M72" s="12">
         <v>6</v>
       </c>
       <c r="N72">
@@ -9198,7 +9210,7 @@
         <v>80</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G73">
         <v>10</v>
@@ -9218,7 +9230,7 @@
       <c r="L73">
         <v>0</v>
       </c>
-      <c r="M73">
+      <c r="M73" s="12">
         <v>0</v>
       </c>
       <c r="N73">
@@ -9299,7 +9311,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G74" s="2">
         <v>10</v>
@@ -9319,7 +9331,7 @@
       <c r="L74" s="2">
         <v>0</v>
       </c>
-      <c r="M74" s="2">
+      <c r="M74" s="15">
         <v>0</v>
       </c>
       <c r="N74" s="2">
@@ -9400,7 +9412,7 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G75">
         <v>30</v>
@@ -9420,7 +9432,7 @@
       <c r="L75">
         <v>1</v>
       </c>
-      <c r="M75">
+      <c r="M75" s="12">
         <v>2</v>
       </c>
       <c r="N75">
@@ -9501,7 +9513,7 @@
         <v>30</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G76">
         <v>30</v>
@@ -9521,7 +9533,7 @@
       <c r="L76">
         <v>0</v>
       </c>
-      <c r="M76">
+      <c r="M76" s="12">
         <v>0</v>
       </c>
       <c r="N76">
@@ -9622,7 +9634,7 @@
       <c r="L77" s="2">
         <v>0</v>
       </c>
-      <c r="M77" s="2">
+      <c r="M77" s="15">
         <v>0</v>
       </c>
       <c r="N77" s="2">
@@ -9703,7 +9715,7 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="G78">
         <v>10</v>
@@ -9723,7 +9735,7 @@
       <c r="L78">
         <v>0</v>
       </c>
-      <c r="M78">
+      <c r="M78" s="12">
         <v>0</v>
       </c>
       <c r="N78">
@@ -9804,7 +9816,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G79" s="2">
         <v>20</v>
@@ -9824,7 +9836,7 @@
       <c r="L79" s="2">
         <v>0</v>
       </c>
-      <c r="M79" s="2">
+      <c r="M79" s="15">
         <v>0</v>
       </c>
       <c r="N79" s="2">
@@ -9925,7 +9937,7 @@
       <c r="L80">
         <v>0</v>
       </c>
-      <c r="M80">
+      <c r="M80" s="12">
         <v>1</v>
       </c>
       <c r="N80">
@@ -10006,7 +10018,7 @@
         <v>40</v>
       </c>
       <c r="F81">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G81">
         <v>15</v>
@@ -10026,7 +10038,7 @@
       <c r="L81">
         <v>0</v>
       </c>
-      <c r="M81">
+      <c r="M81" s="12">
         <v>0</v>
       </c>
       <c r="N81">
@@ -10107,7 +10119,7 @@
         <v>120</v>
       </c>
       <c r="F82">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="G82">
         <v>5</v>
@@ -10127,7 +10139,7 @@
       <c r="L82">
         <v>0</v>
       </c>
-      <c r="M82">
+      <c r="M82" s="12">
         <v>0</v>
       </c>
       <c r="N82">
@@ -10205,7 +10217,7 @@
         <v>80</v>
       </c>
       <c r="F83">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G83">
         <v>20</v>
@@ -10225,7 +10237,7 @@
       <c r="L83">
         <v>0</v>
       </c>
-      <c r="M83">
+      <c r="M83" s="12">
         <v>0</v>
       </c>
       <c r="N83">
@@ -10323,7 +10335,7 @@
       <c r="L84" s="2">
         <v>0</v>
       </c>
-      <c r="M84" s="2">
+      <c r="M84" s="15">
         <v>0</v>
       </c>
       <c r="N84" s="2">
@@ -10424,7 +10436,7 @@
       <c r="L85" s="2">
         <v>0</v>
       </c>
-      <c r="M85" s="2">
+      <c r="M85" s="15">
         <v>0</v>
       </c>
       <c r="N85" s="2">
@@ -10525,7 +10537,7 @@
       <c r="L86" s="2">
         <v>0</v>
       </c>
-      <c r="M86" s="2">
+      <c r="M86" s="15">
         <v>7</v>
       </c>
       <c r="N86" s="2">
@@ -10626,7 +10638,7 @@
       <c r="L87" s="3">
         <v>0</v>
       </c>
-      <c r="M87" s="3">
+      <c r="M87" s="14">
         <v>0</v>
       </c>
       <c r="N87" s="3">
@@ -10727,7 +10739,7 @@
       <c r="L88" s="2">
         <v>0</v>
       </c>
-      <c r="M88" s="2">
+      <c r="M88" s="15">
         <v>0</v>
       </c>
       <c r="N88" s="2">
@@ -10808,7 +10820,7 @@
         <v>-2</v>
       </c>
       <c r="F89" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G89" s="2">
         <v>15</v>
@@ -10828,7 +10840,7 @@
       <c r="L89" s="2">
         <v>0</v>
       </c>
-      <c r="M89" s="2">
+      <c r="M89" s="15">
         <v>0</v>
       </c>
       <c r="N89" s="2">
@@ -10909,7 +10921,7 @@
         <v>40</v>
       </c>
       <c r="F90" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G90" s="2">
         <v>20</v>
@@ -10929,7 +10941,7 @@
       <c r="L90" s="2">
         <v>0</v>
       </c>
-      <c r="M90" s="2">
+      <c r="M90" s="15">
         <v>0</v>
       </c>
       <c r="N90" s="2">
@@ -11010,7 +11022,7 @@
         <v>35</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G91">
         <v>35</v>
@@ -11030,7 +11042,7 @@
       <c r="L91">
         <v>0</v>
       </c>
-      <c r="M91">
+      <c r="M91" s="12">
         <v>0</v>
       </c>
       <c r="N91">
@@ -11108,7 +11120,7 @@
         <v>120</v>
       </c>
       <c r="F92">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G92">
         <v>10</v>
@@ -11128,7 +11140,7 @@
       <c r="L92">
         <v>0</v>
       </c>
-      <c r="M92">
+      <c r="M92" s="12">
         <v>0</v>
       </c>
       <c r="N92">
@@ -11209,7 +11221,7 @@
         <v>25</v>
       </c>
       <c r="F93">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="G93">
         <v>20</v>
@@ -11229,7 +11241,7 @@
       <c r="L93">
         <v>0</v>
       </c>
-      <c r="M93">
+      <c r="M93" s="12">
         <v>0</v>
       </c>
       <c r="N93">
@@ -11310,7 +11322,7 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G94">
         <v>40</v>
@@ -11330,7 +11342,7 @@
       <c r="L94">
         <v>0</v>
       </c>
-      <c r="M94">
+      <c r="M94" s="12">
         <v>0</v>
       </c>
       <c r="N94">
@@ -11411,7 +11423,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="2">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="G95" s="2">
         <v>35</v>
@@ -11431,7 +11443,7 @@
       <c r="L95" s="2">
         <v>0</v>
       </c>
-      <c r="M95" s="2">
+      <c r="M95" s="15">
         <v>0</v>
       </c>
       <c r="N95" s="2">
@@ -11512,7 +11524,7 @@
         <v>15</v>
       </c>
       <c r="F96">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G96">
         <v>35</v>
@@ -11532,7 +11544,7 @@
       <c r="L96">
         <v>0</v>
       </c>
-      <c r="M96">
+      <c r="M96" s="12">
         <v>0</v>
       </c>
       <c r="N96">
@@ -11613,7 +11625,7 @@
         <v>40</v>
       </c>
       <c r="F97">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G97">
         <v>35</v>
@@ -11633,7 +11645,7 @@
       <c r="L97">
         <v>0</v>
       </c>
-      <c r="M97">
+      <c r="M97" s="12">
         <v>0</v>
       </c>
       <c r="N97">
@@ -11711,7 +11723,7 @@
         <v>65</v>
       </c>
       <c r="F98">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G98">
         <v>20</v>
@@ -11731,7 +11743,7 @@
       <c r="L98">
         <v>0</v>
       </c>
-      <c r="M98">
+      <c r="M98" s="12">
         <v>0</v>
       </c>
       <c r="N98">
@@ -11812,7 +11824,7 @@
         <v>90</v>
       </c>
       <c r="F99">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G99">
         <v>10</v>
@@ -11832,7 +11844,7 @@
       <c r="L99">
         <v>1</v>
       </c>
-      <c r="M99">
+      <c r="M99" s="12">
         <v>4</v>
       </c>
       <c r="N99">
@@ -11913,7 +11925,7 @@
         <v>0</v>
       </c>
       <c r="F100" s="5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G100" s="5">
         <v>15</v>
@@ -11933,7 +11945,7 @@
       <c r="L100" s="5">
         <v>0</v>
       </c>
-      <c r="M100" s="5">
+      <c r="M100" s="16">
         <v>0</v>
       </c>
       <c r="N100" s="5">
@@ -12014,7 +12026,7 @@
         <v>40</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G101">
         <v>30</v>
@@ -12034,7 +12046,7 @@
       <c r="L101">
         <v>0</v>
       </c>
-      <c r="M101">
+      <c r="M101" s="12">
         <v>0</v>
       </c>
       <c r="N101">
@@ -12115,7 +12127,7 @@
         <v>20</v>
       </c>
       <c r="F102" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G102" s="3">
         <v>20</v>
@@ -12135,7 +12147,7 @@
       <c r="L102" s="3">
         <v>0</v>
       </c>
-      <c r="M102" s="3">
+      <c r="M102" s="14">
         <v>0</v>
       </c>
       <c r="N102" s="3">
@@ -12216,7 +12228,7 @@
         <v>55</v>
       </c>
       <c r="F103">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="G103">
         <v>25</v>
@@ -12236,7 +12248,7 @@
       <c r="L103">
         <v>0</v>
       </c>
-      <c r="M103">
+      <c r="M103" s="12">
         <v>0</v>
       </c>
       <c r="N103">
@@ -12317,7 +12329,7 @@
         <v>80</v>
       </c>
       <c r="F104" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G104" s="6">
         <v>10</v>
@@ -12337,7 +12349,7 @@
       <c r="L104" s="6">
         <v>0</v>
       </c>
-      <c r="M104" s="6">
+      <c r="M104" s="17">
         <v>0</v>
       </c>
       <c r="N104" s="6">
@@ -12438,7 +12450,7 @@
       <c r="L105">
         <v>0</v>
       </c>
-      <c r="M105">
+      <c r="M105" s="12">
         <v>0</v>
       </c>
       <c r="N105">
@@ -12539,7 +12551,7 @@
       <c r="L106" s="2">
         <v>0</v>
       </c>
-      <c r="M106" s="2">
+      <c r="M106" s="15">
         <v>0</v>
       </c>
       <c r="N106" s="2">
@@ -12640,7 +12652,7 @@
       <c r="L107" s="2">
         <v>0</v>
       </c>
-      <c r="M107" s="2">
+      <c r="M107" s="15">
         <v>0</v>
       </c>
       <c r="N107" s="2">
@@ -12741,7 +12753,7 @@
       <c r="L108" s="2">
         <v>0</v>
       </c>
-      <c r="M108" s="2">
+      <c r="M108" s="15">
         <v>0</v>
       </c>
       <c r="N108" s="2">
@@ -12822,7 +12834,7 @@
         <v>75</v>
       </c>
       <c r="F109">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G109">
         <v>10</v>
@@ -12842,7 +12854,7 @@
       <c r="L109">
         <v>0</v>
       </c>
-      <c r="M109">
+      <c r="M109" s="12">
         <v>0</v>
       </c>
       <c r="N109">
@@ -12923,7 +12935,7 @@
         <v>50</v>
       </c>
       <c r="F110">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G110">
         <v>15</v>
@@ -12943,7 +12955,7 @@
       <c r="L110">
         <v>0</v>
       </c>
-      <c r="M110">
+      <c r="M110" s="12">
         <v>0</v>
       </c>
       <c r="N110">
@@ -13021,7 +13033,7 @@
         <v>60</v>
       </c>
       <c r="F111" s="6">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G111" s="6">
         <v>15</v>
@@ -13041,7 +13053,7 @@
       <c r="L111" s="6">
         <v>0</v>
       </c>
-      <c r="M111" s="6">
+      <c r="M111" s="17">
         <v>0</v>
       </c>
       <c r="N111" s="6">
@@ -13122,7 +13134,7 @@
         <v>0</v>
       </c>
       <c r="F112">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G112">
         <v>15</v>
@@ -13142,7 +13154,7 @@
       <c r="L112">
         <v>1</v>
       </c>
-      <c r="M112">
+      <c r="M112" s="12">
         <v>6</v>
       </c>
       <c r="N112">
@@ -13223,7 +13235,7 @@
         <v>40</v>
       </c>
       <c r="F113">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G113">
         <v>35</v>
@@ -13243,7 +13255,7 @@
       <c r="L113">
         <v>0</v>
       </c>
-      <c r="M113">
+      <c r="M113" s="12">
         <v>0</v>
       </c>
       <c r="N113">
@@ -13321,7 +13333,7 @@
         <v>0</v>
       </c>
       <c r="F114">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G114">
         <v>40</v>
@@ -13341,7 +13353,7 @@
       <c r="L114">
         <v>1</v>
       </c>
-      <c r="M114">
+      <c r="M114" s="12">
         <v>2</v>
       </c>
       <c r="N114">
@@ -13422,7 +13434,7 @@
         <v>-2</v>
       </c>
       <c r="F115" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G115" s="2">
         <v>20</v>
@@ -13442,7 +13454,7 @@
       <c r="L115" s="2">
         <v>0</v>
       </c>
-      <c r="M115" s="2">
+      <c r="M115" s="15">
         <v>0</v>
       </c>
       <c r="N115" s="2">
@@ -13523,7 +13535,7 @@
         <v>200</v>
       </c>
       <c r="F116" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G116" s="2">
         <v>5</v>
@@ -13543,7 +13555,7 @@
       <c r="L116" s="2">
         <v>0</v>
       </c>
-      <c r="M116" s="2">
+      <c r="M116" s="15">
         <v>0</v>
       </c>
       <c r="N116" s="2">
@@ -13644,7 +13656,7 @@
       <c r="L117" s="6">
         <v>0</v>
       </c>
-      <c r="M117" s="6">
+      <c r="M117" s="17">
         <v>1</v>
       </c>
       <c r="N117" s="6">
@@ -13725,7 +13737,7 @@
         <v>0</v>
       </c>
       <c r="F118">
-        <v>0.55000000000000004</v>
+        <v>55</v>
       </c>
       <c r="G118">
         <v>15</v>
@@ -13745,7 +13757,7 @@
       <c r="L118">
         <v>0</v>
       </c>
-      <c r="M118">
+      <c r="M118" s="12">
         <v>0</v>
       </c>
       <c r="N118">
@@ -13826,7 +13838,7 @@
         <v>130</v>
       </c>
       <c r="F119">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G119">
         <v>10</v>
@@ -13846,7 +13858,7 @@
       <c r="L119">
         <v>0</v>
       </c>
-      <c r="M119">
+      <c r="M119" s="12">
         <v>2</v>
       </c>
       <c r="N119">
@@ -13927,7 +13939,7 @@
         <v>140</v>
       </c>
       <c r="F120">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G120">
         <v>5</v>
@@ -13947,7 +13959,7 @@
       <c r="L120">
         <v>0</v>
       </c>
-      <c r="M120">
+      <c r="M120" s="12">
         <v>0</v>
       </c>
       <c r="N120">
@@ -14028,7 +14040,7 @@
         <v>80</v>
       </c>
       <c r="F121">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="G121">
         <v>20</v>
@@ -14048,7 +14060,7 @@
       <c r="L121">
         <v>0</v>
       </c>
-      <c r="M121">
+      <c r="M121" s="12">
         <v>0</v>
       </c>
       <c r="N121">
@@ -14126,7 +14138,7 @@
         <v>70</v>
       </c>
       <c r="F122">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G122">
         <v>20</v>
@@ -14146,7 +14158,7 @@
       <c r="L122">
         <v>0</v>
       </c>
-      <c r="M122">
+      <c r="M122" s="12">
         <v>0</v>
       </c>
       <c r="N122">
@@ -14227,7 +14239,7 @@
         <v>0</v>
       </c>
       <c r="F123">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="G123">
         <v>15</v>
@@ -14247,7 +14259,7 @@
       <c r="L123">
         <v>0</v>
       </c>
-      <c r="M123">
+      <c r="M123" s="12">
         <v>0</v>
       </c>
       <c r="N123">
@@ -14328,7 +14340,7 @@
         <v>65</v>
       </c>
       <c r="F124">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G124">
         <v>20</v>
@@ -14348,7 +14360,7 @@
       <c r="L124">
         <v>0</v>
       </c>
-      <c r="M124">
+      <c r="M124" s="12">
         <v>0</v>
       </c>
       <c r="N124">
@@ -14429,7 +14441,7 @@
         <v>30</v>
       </c>
       <c r="F125">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="G125">
         <v>20</v>
@@ -14449,7 +14461,7 @@
       <c r="L125">
         <v>0</v>
       </c>
-      <c r="M125">
+      <c r="M125" s="12">
         <v>0</v>
       </c>
       <c r="N125">
@@ -14530,7 +14542,7 @@
         <v>0</v>
       </c>
       <c r="F126">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G126">
         <v>20</v>
@@ -14550,7 +14562,7 @@
       <c r="L126">
         <v>1</v>
       </c>
-      <c r="M126">
+      <c r="M126" s="12">
         <v>6</v>
       </c>
       <c r="N126">
@@ -14631,7 +14643,7 @@
         <v>0</v>
       </c>
       <c r="F127">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G127">
         <v>10</v>
@@ -14651,7 +14663,7 @@
       <c r="L127">
         <v>0</v>
       </c>
-      <c r="M127">
+      <c r="M127" s="12">
         <v>0</v>
       </c>
       <c r="N127">
@@ -14732,7 +14744,7 @@
         <v>120</v>
       </c>
       <c r="F128">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G128">
         <v>10</v>
@@ -14752,7 +14764,7 @@
       <c r="L128">
         <v>0</v>
       </c>
-      <c r="M128">
+      <c r="M128" s="12">
         <v>0</v>
       </c>
       <c r="N128">
@@ -14833,7 +14845,7 @@
         <v>20</v>
       </c>
       <c r="F129" s="5">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G129" s="5">
         <v>20</v>
@@ -14853,7 +14865,7 @@
       <c r="L129" s="5">
         <v>0</v>
       </c>
-      <c r="M129" s="5">
+      <c r="M129" s="16">
         <v>0</v>
       </c>
       <c r="N129" s="5">
@@ -14934,7 +14946,7 @@
         <v>20</v>
       </c>
       <c r="F130" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G130" s="6">
         <v>15</v>
@@ -14954,7 +14966,7 @@
       <c r="L130" s="6">
         <v>0</v>
       </c>
-      <c r="M130" s="6">
+      <c r="M130" s="17">
         <v>0</v>
       </c>
       <c r="N130" s="6">
@@ -15055,7 +15067,7 @@
       <c r="L131" s="2">
         <v>0</v>
       </c>
-      <c r="M131" s="2">
+      <c r="M131" s="15">
         <v>0</v>
       </c>
       <c r="N131" s="2">
@@ -15136,7 +15148,7 @@
         <v>0</v>
       </c>
       <c r="F132">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G132">
         <v>15</v>
@@ -15156,7 +15168,7 @@
       <c r="L132">
         <v>0</v>
       </c>
-      <c r="M132">
+      <c r="M132" s="12">
         <v>0</v>
       </c>
       <c r="N132">
@@ -15237,7 +15249,7 @@
         <v>65</v>
       </c>
       <c r="F133" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G133" s="2">
         <v>20</v>
@@ -15257,7 +15269,7 @@
       <c r="L133" s="2">
         <v>0</v>
       </c>
-      <c r="M133" s="2">
+      <c r="M133" s="15">
         <v>0</v>
       </c>
       <c r="N133" s="2">
@@ -15338,7 +15350,7 @@
         <v>80</v>
       </c>
       <c r="F134">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G134">
         <v>15</v>
@@ -15358,7 +15370,7 @@
       <c r="L134">
         <v>0</v>
       </c>
-      <c r="M134">
+      <c r="M134" s="12">
         <v>0</v>
       </c>
       <c r="N134">
@@ -15436,7 +15448,7 @@
         <v>0</v>
       </c>
       <c r="F135">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="G135">
         <v>40</v>
@@ -15456,7 +15468,7 @@
       <c r="L135">
         <v>1</v>
       </c>
-      <c r="M135">
+      <c r="M135" s="12">
         <v>5</v>
       </c>
       <c r="N135">
@@ -15537,7 +15549,7 @@
         <v>50</v>
       </c>
       <c r="F136">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G136">
         <v>1</v>
@@ -15557,7 +15569,7 @@
       <c r="L136">
         <v>0</v>
       </c>
-      <c r="M136">
+      <c r="M136" s="12">
         <v>0</v>
       </c>
       <c r="N136">
@@ -15638,7 +15650,7 @@
         <v>0</v>
       </c>
       <c r="F137">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="G137">
         <v>30</v>
@@ -15658,7 +15670,7 @@
       <c r="L137">
         <v>0</v>
       </c>
-      <c r="M137">
+      <c r="M137" s="12">
         <v>0</v>
       </c>
       <c r="N137">
@@ -15739,7 +15751,7 @@
         <v>80</v>
       </c>
       <c r="F138">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="G138">
         <v>20</v>
@@ -15759,7 +15771,7 @@
       <c r="L138">
         <v>0</v>
       </c>
-      <c r="M138">
+      <c r="M138" s="12">
         <v>0</v>
       </c>
       <c r="N138">
@@ -15860,7 +15872,7 @@
       <c r="L139" s="2">
         <v>0</v>
       </c>
-      <c r="M139" s="2">
+      <c r="M139" s="15">
         <v>0</v>
       </c>
       <c r="N139" s="2">
@@ -15941,7 +15953,7 @@
         <v>0</v>
       </c>
       <c r="F140" s="2">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G140" s="2">
         <v>10</v>
@@ -15961,7 +15973,7 @@
       <c r="L140" s="2">
         <v>0</v>
       </c>
-      <c r="M140" s="2">
+      <c r="M140" s="15">
         <v>0</v>
       </c>
       <c r="N140" s="2">
@@ -16042,7 +16054,7 @@
         <v>0</v>
       </c>
       <c r="F141">
-        <v>0.55000000000000004</v>
+        <v>55</v>
       </c>
       <c r="G141">
         <v>20</v>
@@ -16062,7 +16074,7 @@
       <c r="L141">
         <v>0</v>
       </c>
-      <c r="M141">
+      <c r="M141" s="12">
         <v>0</v>
       </c>
       <c r="N141">
@@ -16143,7 +16155,7 @@
         <v>90</v>
       </c>
       <c r="F142">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G142">
         <v>15</v>
@@ -16163,7 +16175,7 @@
       <c r="L142">
         <v>0</v>
       </c>
-      <c r="M142">
+      <c r="M142" s="12">
         <v>0</v>
       </c>
       <c r="N142">
@@ -16244,7 +16256,7 @@
         <v>60</v>
       </c>
       <c r="F143" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G143" s="2">
         <v>20</v>
@@ -16264,7 +16276,7 @@
       <c r="L143" s="2">
         <v>0</v>
       </c>
-      <c r="M143" s="2">
+      <c r="M143" s="15">
         <v>0</v>
       </c>
       <c r="N143" s="2">
@@ -16365,7 +16377,7 @@
       <c r="L144">
         <v>0</v>
       </c>
-      <c r="M144">
+      <c r="M144" s="12">
         <v>1</v>
       </c>
       <c r="N144">
@@ -16446,7 +16458,7 @@
         <v>40</v>
       </c>
       <c r="F145">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G145">
         <v>35</v>
@@ -16466,7 +16478,7 @@
       <c r="L145">
         <v>0</v>
       </c>
-      <c r="M145">
+      <c r="M145" s="12">
         <v>0</v>
       </c>
       <c r="N145">
@@ -16544,7 +16556,7 @@
         <v>0</v>
       </c>
       <c r="F146">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G146">
         <v>30</v>
@@ -16564,7 +16576,7 @@
       <c r="L146">
         <v>1</v>
       </c>
-      <c r="M146">
+      <c r="M146" s="12">
         <v>2</v>
       </c>
       <c r="N146">
@@ -16645,7 +16657,7 @@
         <v>90</v>
       </c>
       <c r="F147">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="G147">
         <v>20</v>
@@ -16665,7 +16677,7 @@
       <c r="L147">
         <v>0</v>
       </c>
-      <c r="M147">
+      <c r="M147" s="12">
         <v>0</v>
       </c>
       <c r="N147">
@@ -16766,7 +16778,7 @@
       <c r="L148" s="2">
         <v>0</v>
       </c>
-      <c r="M148" s="2">
+      <c r="M148" s="15">
         <v>0</v>
       </c>
       <c r="N148" s="2">
@@ -16847,7 +16859,7 @@
         <v>120</v>
       </c>
       <c r="F149">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G149">
         <v>10</v>
@@ -16867,7 +16879,7 @@
       <c r="L149">
         <v>0</v>
       </c>
-      <c r="M149">
+      <c r="M149" s="12">
         <v>0</v>
       </c>
       <c r="N149">
@@ -16925,7 +16937,7 @@
         <v>3</v>
       </c>
       <c r="AF149" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AG149" t="s">
         <v>168</v>
@@ -16951,7 +16963,7 @@
         <v>110</v>
       </c>
       <c r="F150">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="G150">
         <v>10</v>
@@ -16971,7 +16983,7 @@
       <c r="L150">
         <v>0</v>
       </c>
-      <c r="M150">
+      <c r="M150" s="12">
         <v>0</v>
       </c>
       <c r="N150">
@@ -17052,7 +17064,7 @@
         <v>75</v>
       </c>
       <c r="F151">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G151">
         <v>15</v>
@@ -17072,7 +17084,7 @@
       <c r="L151">
         <v>0</v>
       </c>
-      <c r="M151">
+      <c r="M151" s="12">
         <v>0</v>
       </c>
       <c r="N151">
@@ -17153,7 +17165,7 @@
         <v>40</v>
       </c>
       <c r="F152">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G152">
         <v>30</v>
@@ -17173,7 +17185,7 @@
       <c r="L152">
         <v>0</v>
       </c>
-      <c r="M152">
+      <c r="M152" s="12">
         <v>0</v>
       </c>
       <c r="N152">
@@ -17254,7 +17266,7 @@
         <v>0</v>
       </c>
       <c r="F153">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G153">
         <v>20</v>
@@ -17274,7 +17286,7 @@
       <c r="L153">
         <v>0</v>
       </c>
-      <c r="M153">
+      <c r="M153" s="12">
         <v>0</v>
       </c>
       <c r="N153">
@@ -17355,7 +17367,7 @@
         <v>90</v>
       </c>
       <c r="F154" s="8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G154">
         <v>15</v>
@@ -17375,7 +17387,7 @@
       <c r="L154">
         <v>0</v>
       </c>
-      <c r="M154">
+      <c r="M154" s="12">
         <v>0</v>
       </c>
       <c r="N154">
@@ -17456,7 +17468,7 @@
         <v>0</v>
       </c>
       <c r="F155" s="2">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G155" s="2">
         <v>10</v>
@@ -17476,7 +17488,7 @@
       <c r="L155" s="2">
         <v>0</v>
       </c>
-      <c r="M155" s="2">
+      <c r="M155" s="15">
         <v>0</v>
       </c>
       <c r="N155" s="2">
@@ -17577,7 +17589,7 @@
       <c r="L156" s="2">
         <v>0</v>
       </c>
-      <c r="M156" s="2">
+      <c r="M156" s="15">
         <v>0</v>
       </c>
       <c r="N156" s="2">
@@ -17658,7 +17670,7 @@
         <v>80</v>
       </c>
       <c r="F157" s="10">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G157" s="10">
         <v>10</v>
@@ -17678,7 +17690,7 @@
       <c r="L157" s="10">
         <v>0</v>
       </c>
-      <c r="M157" s="10">
+      <c r="M157" s="19">
         <v>0</v>
       </c>
       <c r="N157" s="10">
@@ -17759,7 +17771,7 @@
         <v>25</v>
       </c>
       <c r="F158" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G158" s="6">
         <v>20</v>
@@ -17779,7 +17791,7 @@
       <c r="L158" s="6">
         <v>0</v>
       </c>
-      <c r="M158" s="6">
+      <c r="M158" s="17">
         <v>0</v>
       </c>
       <c r="N158" s="6">
@@ -17860,7 +17872,7 @@
         <v>45</v>
       </c>
       <c r="F159">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G159">
         <v>25</v>
@@ -17880,7 +17892,7 @@
       <c r="L159">
         <v>0</v>
       </c>
-      <c r="M159">
+      <c r="M159" s="12">
         <v>0</v>
       </c>
       <c r="N159">
@@ -17958,7 +17970,7 @@
         <v>55</v>
       </c>
       <c r="F160">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G160">
         <v>30</v>
@@ -17978,7 +17990,7 @@
       <c r="L160">
         <v>0</v>
       </c>
-      <c r="M160">
+      <c r="M160" s="12">
         <v>0</v>
       </c>
       <c r="N160">
@@ -18056,7 +18068,7 @@
         <v>40</v>
       </c>
       <c r="F161">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G161">
         <v>25</v>
@@ -18076,7 +18088,7 @@
       <c r="L161">
         <v>0</v>
       </c>
-      <c r="M161">
+      <c r="M161" s="12">
         <v>0</v>
       </c>
       <c r="N161">
@@ -18154,7 +18166,7 @@
         <v>80</v>
       </c>
       <c r="F162">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G162">
         <v>15</v>
@@ -18174,7 +18186,7 @@
       <c r="L162">
         <v>0</v>
       </c>
-      <c r="M162">
+      <c r="M162" s="12">
         <v>0</v>
       </c>
       <c r="N162">
@@ -18275,7 +18287,7 @@
       <c r="L163" s="2">
         <v>0</v>
       </c>
-      <c r="M163" s="2">
+      <c r="M163" s="15">
         <v>0</v>
       </c>
       <c r="N163" s="2">
@@ -18356,7 +18368,7 @@
         <v>60</v>
       </c>
       <c r="F164">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G164">
         <v>35</v>
@@ -18376,7 +18388,7 @@
       <c r="L164">
         <v>0</v>
       </c>
-      <c r="M164">
+      <c r="M164" s="12">
         <v>0</v>
       </c>
       <c r="N164">
@@ -18474,7 +18486,7 @@
       <c r="L165">
         <v>0</v>
       </c>
-      <c r="M165">
+      <c r="M165" s="12">
         <v>2</v>
       </c>
       <c r="N165">
@@ -18555,7 +18567,7 @@
         <v>15</v>
       </c>
       <c r="F166" s="2">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="G166" s="2">
         <v>20</v>
@@ -18575,7 +18587,7 @@
       <c r="L166" s="2">
         <v>0</v>
       </c>
-      <c r="M166" s="2">
+      <c r="M166" s="15">
         <v>0</v>
       </c>
       <c r="N166" s="2">
@@ -18633,7 +18645,7 @@
         <v>5</v>
       </c>
       <c r="AF166" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AG166" s="2" t="s">
         <v>48</v>

</xml_diff>